<commit_message>
Added updated SPI Wrapper project files
</commit_message>
<xml_diff>
--- a/Verification_Plan.xlsx
+++ b/Verification_Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital_Verification_Diploma\SPI_Single_Port_RAM_Verification_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\githup_repo\SPISLAVE_uvm\SPI_Single_Port_RAM_Verification_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5661BAC-6522-4976-B8F5-EE3C5AAD29D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03145F03-3F9D-40F5-8D63-9C96D5F95070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2CDF5C61-3800-429E-9FAE-2518D1565771}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Label</t>
   </si>
@@ -85,6 +85,42 @@
   </si>
   <si>
     <t>If rx_valid is asserted and din[9:8] is 10, read address register should be written to din[7:0]. If din[9:8] is 11, dout should be read from memory address of rd_address</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>When reset is asserted , MISO , rx_data , rx_valid will be low</t>
+  </si>
+  <si>
+    <t>Directed at the beginning of simulation then randomized</t>
+  </si>
+  <si>
+    <t>SS_n for all cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assertions </t>
+  </si>
+  <si>
+    <t>SS_n for  read_data</t>
+  </si>
+  <si>
+    <t>tx_valid for read data</t>
+  </si>
+  <si>
+    <t>when the least significant bit [0:2]of array_rand inside {111} and counter not equal 24 , SS_n will be low and if equal will be high</t>
+  </si>
+  <si>
+    <t>when the least significant bit [0:2]of array_rand inside {000,001,110} and counter not equal 14 , SS_n will be low and if equal will be high</t>
+  </si>
+  <si>
+    <t>when the least significant bit [0:2]of array_rand equal 3'b111 and counter equal 23 , then tx_valid will be asserted</t>
+  </si>
+  <si>
+    <t>array_rand for all cases</t>
+  </si>
+  <si>
+    <t>if SS_n fell ,  the least significant bit [0:2]of array_rand will be inside {000,001,110,111}</t>
   </si>
 </sst>
 </file>
@@ -152,13 +188,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,14 +536,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1313A1F-0A01-4585-AC2F-99D26BA555E1}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
     <col min="2" max="2" width="41.77734375" customWidth="1"/>
     <col min="3" max="3" width="33.44140625" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
@@ -552,6 +595,9 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
@@ -566,6 +612,9 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
@@ -580,8 +629,96 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
       <c r="E5" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>